<commit_message>
firsttime submit to tomcat version
</commit_message>
<xml_diff>
--- a/chinaproject/资料/Type of service - china.xlsx
+++ b/chinaproject/资料/Type of service - china.xlsx
@@ -88,91 +88,91 @@
     <t>fixed rate</t>
   </si>
   <si>
+    <t>非绑定服务</t>
+  </si>
+  <si>
+    <t>叫车服务</t>
+  </si>
+  <si>
+    <t>fixed fee</t>
+  </si>
+  <si>
+    <t>购买机票服务</t>
+  </si>
+  <si>
+    <t>申请驾照服务</t>
+  </si>
+  <si>
+    <t>驾驶培训</t>
+  </si>
+  <si>
+    <t>快递业务</t>
+  </si>
+  <si>
+    <t>陪同考驾照服务</t>
+  </si>
+  <si>
+    <t>另类服务</t>
+  </si>
+  <si>
+    <t>英语私教</t>
+  </si>
+  <si>
+    <t>搬家服务</t>
+  </si>
+  <si>
+    <t>subcontract</t>
+  </si>
+  <si>
+    <t>代驾服务</t>
+  </si>
+  <si>
+    <t>家政服务</t>
+  </si>
+  <si>
+    <t>扫雪服务</t>
+  </si>
+  <si>
+    <t>除草服务</t>
+  </si>
+  <si>
+    <t>翻译服务（书面，陪同）</t>
+  </si>
+  <si>
+    <t>购买/安装家具服务</t>
+  </si>
+  <si>
+    <t>购车服务</t>
+  </si>
+  <si>
+    <t>旅游服务</t>
+  </si>
+  <si>
+    <t>陪读服务</t>
+  </si>
+  <si>
+    <t>活动聚会</t>
+  </si>
+  <si>
+    <t>开除紧急处理</t>
+  </si>
+  <si>
+    <t>hourlyrate</t>
+  </si>
+  <si>
+    <t>转学申请</t>
+  </si>
+  <si>
+    <t>美国生活热线</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>服务信息交流</t>
+  </si>
+  <si>
     <t>公司咨询服务</t>
-  </si>
-  <si>
-    <t>非绑定服务</t>
-  </si>
-  <si>
-    <t>叫车服务</t>
-  </si>
-  <si>
-    <t>fixed fee</t>
-  </si>
-  <si>
-    <t>购买机票服务</t>
-  </si>
-  <si>
-    <t>申请驾照服务</t>
-  </si>
-  <si>
-    <t>驾驶培训</t>
-  </si>
-  <si>
-    <t>快递业务</t>
-  </si>
-  <si>
-    <t>陪同考驾照服务</t>
-  </si>
-  <si>
-    <t>另类服务</t>
-  </si>
-  <si>
-    <t>英语私教</t>
-  </si>
-  <si>
-    <t>搬家服务</t>
-  </si>
-  <si>
-    <t>subcontract</t>
-  </si>
-  <si>
-    <t>代驾服务</t>
-  </si>
-  <si>
-    <t>家政服务</t>
-  </si>
-  <si>
-    <t>扫雪服务</t>
-  </si>
-  <si>
-    <t>除草服务</t>
-  </si>
-  <si>
-    <t>翻译服务（书面，陪同）</t>
-  </si>
-  <si>
-    <t>购买/安装家具服务</t>
-  </si>
-  <si>
-    <t>购车服务</t>
-  </si>
-  <si>
-    <t>旅游服务</t>
-  </si>
-  <si>
-    <t>陪读服务</t>
-  </si>
-  <si>
-    <t>活动聚会</t>
-  </si>
-  <si>
-    <t>开除紧急处理</t>
-  </si>
-  <si>
-    <t>hourlyrate</t>
-  </si>
-  <si>
-    <t>转学申请</t>
-  </si>
-  <si>
-    <t>美国生活热线</t>
-  </si>
-  <si>
-    <t>????</t>
-  </si>
-  <si>
-    <t>服务信息交流</t>
   </si>
 </sst>
 </file>
@@ -180,12 +180,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,12 +212,28 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,29 +283,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -360,7 +353,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,6 +374,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -460,30 +483,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,6 +571,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -590,15 +613,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -610,21 +624,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -674,163 +673,165 @@
     </border>
   </borders>
   <cellStyleXfs count="50">
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="49" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="49" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="49" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="49" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="49" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1146,10 +1147,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -1189,7 +1190,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1"/>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
@@ -1207,7 +1208,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1"/>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
@@ -1270,10 +1271,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1324,73 +1325,67 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1"/>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:1">
       <c r="A20" s="1"/>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>26</v>
-      </c>
-      <c r="C21" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1"/>
-      <c r="B22" t="s">
-        <v>28</v>
+      <c r="B22" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1"/>
-      <c r="B23" t="s">
-        <v>29</v>
+      <c r="B23" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1"/>
-      <c r="B24" t="s">
-        <v>30</v>
+      <c r="B24" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1"/>
-      <c r="B25" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>27</v>
+      <c r="B25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1"/>
-      <c r="B26" t="s">
-        <v>32</v>
+      <c r="B26" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -1398,10 +1393,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>34</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1409,17 +1404,17 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1"/>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
         <v>35</v>
-      </c>
-      <c r="C28" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1"/>
-      <c r="B29" t="s">
-        <v>37</v>
+      <c r="B29" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -1427,8 +1422,8 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1"/>
-      <c r="B30" t="s">
-        <v>38</v>
+      <c r="B30" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -1436,26 +1431,26 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1"/>
-      <c r="B31" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>36</v>
+      <c r="B31" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1"/>
-      <c r="B32" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>36</v>
+      <c r="B32" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1"/>
-      <c r="B33" t="s">
-        <v>41</v>
+      <c r="B33" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -1463,8 +1458,8 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1"/>
-      <c r="B34" t="s">
-        <v>42</v>
+      <c r="B34" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -1472,8 +1467,8 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1"/>
-      <c r="B35" t="s">
-        <v>43</v>
+      <c r="B35" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -1481,8 +1476,8 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1"/>
-      <c r="B36" t="s">
-        <v>44</v>
+      <c r="B36" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -1490,8 +1485,8 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1"/>
-      <c r="B37" t="s">
-        <v>45</v>
+      <c r="B37" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -1499,8 +1494,8 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1"/>
-      <c r="B38" t="s">
-        <v>46</v>
+      <c r="B38" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -1508,17 +1503,17 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1"/>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1"/>
-      <c r="B40" t="s">
-        <v>49</v>
+      <c r="B40" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -1526,20 +1521,28 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1"/>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" t="s">
         <v>50</v>
-      </c>
-      <c r="C41" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1"/>
       <c r="B42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C42" t="s">
-        <v>51</v>
+      <c r="C43" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>